<commit_message>
excel sheet change for api
</commit_message>
<xml_diff>
--- a/mysite/Url.xlsx
+++ b/mysite/Url.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>EndPoint</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>password: admin</t>
+  </si>
+  <si>
+    <t>Admin Url: https://djangotask.herokuapp.com/admin/</t>
   </si>
 </sst>
 </file>
@@ -193,7 +196,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -214,6 +217,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -522,7 +528,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,7 +540,7 @@
     <col min="5" max="5" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>33</v>
       </c>
@@ -543,6 +549,9 @@
       </c>
       <c r="C1" s="8" t="s">
         <v>35</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -706,8 +715,9 @@
     <hyperlink ref="B11" r:id="rId8"/>
     <hyperlink ref="B12" r:id="rId9"/>
     <hyperlink ref="E12" r:id="rId10"/>
+    <hyperlink ref="D1" r:id="rId11" display="https://djangotask.herokuapp.com/admin/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId11"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>